<commit_message>
Added code for Lab5
Made robot able to localize, identify object, drive towards object,
check if it is a block. If block, grab it, and take to end!
</commit_message>
<xml_diff>
--- a/Lab 4 - Localization/Data.xlsx
+++ b/Lab 4 - Localization/Data.xlsx
@@ -19,15 +19,50 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>Falling Edge</t>
+  </si>
+  <si>
+    <t>Rising Edge</t>
+  </si>
+  <si>
+    <t>Rising Edge Error (deg)</t>
+  </si>
+  <si>
+    <t>Falling Edge Error (deg)</t>
+  </si>
+  <si>
+    <t>Mean (deg)</t>
+  </si>
+  <si>
+    <t>Standard Deviation (deg)</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -50,13 +85,33 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="11">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -386,96 +441,166 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="E1" sqref="E1:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="5" max="5" width="21.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:3">
+    <row r="1" spans="1:7">
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>4.3</v>
       </c>
+      <c r="B2">
+        <v>4.3</v>
+      </c>
       <c r="C2">
         <v>-12</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <f>AVERAGE(B2:B11)</f>
+        <v>1.6300000000000001</v>
+      </c>
+      <c r="G2">
+        <f>AVERAGE(C2:C11)</f>
+        <v>-11.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>3.2</v>
       </c>
+      <c r="B3">
+        <v>3.2</v>
+      </c>
       <c r="C3">
         <v>-16</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <f>STDEV(B2:B11)</f>
+        <v>1.8726392545756854</v>
+      </c>
+      <c r="G3">
+        <f>STDEV(C2:C11)</f>
+        <v>3.1287200080686159</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>-0.1</v>
       </c>
+      <c r="B4">
+        <v>-0.1</v>
+      </c>
       <c r="C4">
         <v>-9</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>2.5</v>
       </c>
+      <c r="B5">
+        <v>2.5</v>
+      </c>
       <c r="C5">
         <v>-8</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>1.8</v>
       </c>
+      <c r="B6">
+        <v>1.8</v>
+      </c>
       <c r="C6">
         <v>-14</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>-2.5</v>
       </c>
+      <c r="B7">
+        <v>-2.5</v>
+      </c>
       <c r="C7">
         <v>-11</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>1.3</v>
       </c>
+      <c r="B8">
+        <v>1.3</v>
+      </c>
       <c r="C8">
         <v>-9</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>2.6</v>
       </c>
+      <c r="B9">
+        <v>2.6</v>
+      </c>
       <c r="C9">
         <v>-12</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>1.8</v>
       </c>
+      <c r="B10">
+        <v>1.8</v>
+      </c>
       <c r="C10">
         <v>-17</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>1.4</v>
       </c>
+      <c r="B11">
+        <v>1.4</v>
+      </c>
       <c r="C11">
         <v>-9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>